<commit_message>
Excel & POM updated
</commit_message>
<xml_diff>
--- a/testdata/OpenEMRData.xlsx
+++ b/testdata/OpenEMRData.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Training\JavaSelenium\OpenEMRApplication\testdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{13EB0AAE-A5A9-4DEA-B6A6-D02834CDC27D}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FA446D17-7701-4858-B760-4A6854F46A4C}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1500" yWindow="1500" windowWidth="17280" windowHeight="8964" xr2:uid="{74573533-2B7D-42D5-93C3-552848841D1D}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{74573533-2B7D-42D5-93C3-552848841D1D}"/>
   </bookViews>
   <sheets>
     <sheet name="validCredentialsTestData" sheetId="1" r:id="rId1"/>
@@ -67,19 +67,13 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color rgb="FF212529"/>
-      <name val="Segoe UI"/>
-      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -102,9 +96,8 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -419,10 +412,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{917E5AE1-DFD9-4FD7-B10B-2EFF10D9B63A}">
-  <dimension ref="A1:D6"/>
+  <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5:XFD8"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -487,14 +480,6 @@
         <v>8</v>
       </c>
     </row>
-    <row r="5" spans="1:4" ht="15" x14ac:dyDescent="0.35">
-      <c r="A5" s="1"/>
-      <c r="B5" s="1"/>
-    </row>
-    <row r="6" spans="1:4" ht="15" x14ac:dyDescent="0.35">
-      <c r="A6" s="1"/>
-      <c r="B6" s="1"/>
-    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>